<commit_message>
update with fixed statistical uncertainties
</commit_message>
<xml_diff>
--- a/pidis/expdata/80096.xlsx
+++ b/pidis/expdata/80096.xlsx
@@ -2826,7 +2826,7 @@
         <v>401</v>
       </c>
       <c r="M2">
-        <v>3.512907379896741e-06</v>
+        <v>0.0002643013856107936</v>
       </c>
       <c r="N2">
         <v>1.993712392307671e-05</v>
@@ -4028,7 +4028,7 @@
         <v>401</v>
       </c>
       <c r="M3">
-        <v>1.299810194568056e-06</v>
+        <v>8.738379411115402e-05</v>
       </c>
       <c r="N3">
         <v>1.392432823447741e-05</v>
@@ -5230,7 +5230,7 @@
         <v>401</v>
       </c>
       <c r="M4">
-        <v>2.167369280540775e-06</v>
+        <v>0.0001094797634897073</v>
       </c>
       <c r="N4">
         <v>2.720840268758233e-05</v>
@@ -6432,7 +6432,7 @@
         <v>401</v>
       </c>
       <c r="M5">
-        <v>5.571294138389145e-07</v>
+        <v>3.565138346917022e-05</v>
       </c>
       <c r="N5">
         <v>1.053320787744128e-05</v>
@@ -7634,7 +7634,7 @@
         <v>401</v>
       </c>
       <c r="M6">
-        <v>8.759880410637838e-07</v>
+        <v>4.533472396518072e-05</v>
       </c>
       <c r="N6">
         <v>2.101188217120237e-05</v>
@@ -8836,7 +8836,7 @@
         <v>401</v>
       </c>
       <c r="M7">
-        <v>2.702615717066203e-07</v>
+        <v>2.318760779456991e-05</v>
       </c>
       <c r="N7">
         <v>8.53189094742297e-06</v>
@@ -10038,7 +10038,7 @@
         <v>401</v>
       </c>
       <c r="M8">
-        <v>4.139543473093811e-07</v>
+        <v>3.031856910183338e-05</v>
       </c>
       <c r="N8">
         <v>1.770042894792863e-05</v>
@@ -11240,7 +11240,7 @@
         <v>401</v>
       </c>
       <c r="M9">
-        <v>6.553354967084828e-07</v>
+        <v>4.360784102504619e-05</v>
       </c>
       <c r="N9">
         <v>4.166185343732862e-05</v>
@@ -12442,7 +12442,7 @@
         <v>401</v>
       </c>
       <c r="M10">
-        <v>1.451289059962464e-07</v>
+        <v>1.834916361378374e-05</v>
       </c>
       <c r="N10">
         <v>7.300584603916689e-06</v>
@@ -13644,7 +13644,7 @@
         <v>401</v>
       </c>
       <c r="M11">
-        <v>2.201042252426695e-07</v>
+        <v>2.477893402450552e-05</v>
       </c>
       <c r="N11">
         <v>1.585754749739128e-05</v>
@@ -14846,7 +14846,7 @@
         <v>401</v>
       </c>
       <c r="M12">
-        <v>3.407062876108197e-07</v>
+        <v>3.612505248530016e-05</v>
       </c>
       <c r="N12">
         <v>3.773309985535159e-05</v>
@@ -16048,7 +16048,7 @@
         <v>401</v>
       </c>
       <c r="M13">
-        <v>5.196062335449928e-07</v>
+        <v>5.371848351378758e-05</v>
       </c>
       <c r="N13">
         <v>9.918883073811145e-05</v>
@@ -17250,7 +17250,7 @@
         <v>401</v>
       </c>
       <c r="M14">
-        <v>8.459405645901169e-08</v>
+        <v>1.633204150158481e-05</v>
       </c>
       <c r="N14">
         <v>6.527197244426255e-06</v>
@@ -18452,7 +18452,7 @@
         <v>401</v>
       </c>
       <c r="M15">
-        <v>1.268162965790221e-07</v>
+        <v>2.270021856269615e-05</v>
       </c>
       <c r="N15">
         <v>1.479715548042529e-05</v>
@@ -19654,7 +19654,7 @@
         <v>401</v>
       </c>
       <c r="M16">
-        <v>1.923661765902568e-07</v>
+        <v>3.343195224501487e-05</v>
       </c>
       <c r="N16">
         <v>3.587798516102814e-05</v>
@@ -20856,7 +20856,7 @@
         <v>401</v>
       </c>
       <c r="M17">
-        <v>2.972122179175441e-07</v>
+        <v>5.126291516023668e-05</v>
       </c>
       <c r="N17">
         <v>9.307713277247653e-05</v>
@@ -22058,7 +22058,7 @@
         <v>401</v>
       </c>
       <c r="M18">
-        <v>5.231171991727571e-08</v>
+        <v>1.575020722295301e-05</v>
       </c>
       <c r="N18">
         <v>6.043713801058382e-06</v>
@@ -23260,7 +23260,7 @@
         <v>401</v>
       </c>
       <c r="M19">
-        <v>7.655039697844359e-08</v>
+        <v>2.233276341625657e-05</v>
       </c>
       <c r="N19">
         <v>1.418024453677607e-05</v>
@@ -24462,7 +24462,7 @@
         <v>401</v>
       </c>
       <c r="M20">
-        <v>1.140921742032956e-07</v>
+        <v>3.321256974721872e-05</v>
       </c>
       <c r="N20">
         <v>3.512946595931012e-05</v>
@@ -25664,7 +25664,7 @@
         <v>401</v>
       </c>
       <c r="M21">
-        <v>1.742561493890708e-07</v>
+        <v>5.100915786550421e-05</v>
       </c>
       <c r="N21">
         <v>9.081342312787204e-05</v>
@@ -26866,7 +26866,7 @@
         <v>401</v>
       </c>
       <c r="M22">
-        <v>2.758152126301555e-07</v>
+        <v>8.153939603533073e-05</v>
       </c>
       <c r="N22">
         <v>0.0002494631048032198</v>
@@ -28068,7 +28068,7 @@
         <v>401</v>
       </c>
       <c r="M23">
-        <v>3.266561379350812e-08</v>
+        <v>1.583946945690012e-05</v>
       </c>
       <c r="N23">
         <v>5.653433255903397e-06</v>
@@ -29270,7 +29270,7 @@
         <v>401</v>
       </c>
       <c r="M24">
-        <v>4.637153728965388e-08</v>
+        <v>2.277473675157797e-05</v>
       </c>
       <c r="N24">
         <v>1.36783357088372e-05</v>
@@ -30472,7 +30472,7 @@
         <v>401</v>
       </c>
       <c r="M25">
-        <v>6.837671677819983e-08</v>
+        <v>3.420807824752051e-05</v>
       </c>
       <c r="N25">
         <v>3.46763861781458e-05</v>
@@ -31674,7 +31674,7 @@
         <v>401</v>
       </c>
       <c r="M26">
-        <v>1.039575945613013e-07</v>
+        <v>5.267925517921627e-05</v>
       </c>
       <c r="N26">
         <v>9.013382250663034e-05</v>
@@ -32876,7 +32876,7 @@
         <v>401</v>
       </c>
       <c r="M27">
-        <v>1.638642007956629e-07</v>
+        <v>8.415489187291594e-05</v>
       </c>
       <c r="N27">
         <v>0.0002431541489716509</v>
@@ -34078,7 +34078,7 @@
         <v>401</v>
       </c>
       <c r="M28">
-        <v>1.916043611517616e-08</v>
+        <v>1.585889994079226e-05</v>
       </c>
       <c r="N28">
         <v>5.119879929297187e-06</v>
@@ -35280,7 +35280,7 @@
         <v>401</v>
       </c>
       <c r="M29">
-        <v>2.700496727107726e-08</v>
+        <v>2.326765084113112e-05</v>
       </c>
       <c r="N29">
         <v>1.291132382120527e-05</v>
@@ -36482,7 +36482,7 @@
         <v>401</v>
       </c>
       <c r="M30">
-        <v>4.018420191754548e-08</v>
+        <v>3.54868665972202e-05</v>
       </c>
       <c r="N30">
         <v>3.365305123160317e-05</v>
@@ -37684,7 +37684,7 @@
         <v>401</v>
       </c>
       <c r="M31">
-        <v>6.164072730859638e-08</v>
+        <v>5.508888805897084e-05</v>
       </c>
       <c r="N31">
         <v>8.840710095443235e-05</v>
@@ -38886,7 +38886,7 @@
         <v>401</v>
       </c>
       <c r="M32">
-        <v>9.696662558957857e-08</v>
+        <v>8.756153224878434e-05</v>
       </c>
       <c r="N32">
         <v>0.0002364939230787262</v>
@@ -40088,7 +40088,7 @@
         <v>401</v>
       </c>
       <c r="M33">
-        <v>1.583236867511349e-07</v>
+        <v>0.0001438636389844995</v>
       </c>
       <c r="N33">
         <v>0.0006592749355147009</v>
@@ -41290,7 +41290,7 @@
         <v>401</v>
       </c>
       <c r="M34">
-        <v>1.044737841724386e-08</v>
+        <v>1.56584089162888e-05</v>
       </c>
       <c r="N34">
         <v>4.459433011680774e-06</v>
@@ -42492,7 +42492,7 @@
         <v>401</v>
       </c>
       <c r="M35">
-        <v>1.520451869268114e-08</v>
+        <v>2.359886047116136e-05</v>
       </c>
       <c r="N35">
         <v>1.179516725970207e-05</v>
@@ -43694,7 +43694,7 @@
         <v>401</v>
       </c>
       <c r="M36">
-        <v>2.324733047645158e-08</v>
+        <v>3.663010848027241e-05</v>
       </c>
       <c r="N36">
         <v>3.147619126518955e-05</v>
@@ -44896,7 +44896,7 @@
         <v>401</v>
       </c>
       <c r="M37">
-        <v>3.631199743655268e-08</v>
+        <v>5.750449829352703e-05</v>
       </c>
       <c r="N37">
         <v>8.333518555637314e-05</v>
@@ -46098,7 +46098,7 @@
         <v>401</v>
       </c>
       <c r="M38">
-        <v>5.755658555826918e-08</v>
+        <v>9.147604070570671e-05</v>
       </c>
       <c r="N38">
         <v>0.0002217734190123689</v>
@@ -47300,7 +47300,7 @@
         <v>401</v>
       </c>
       <c r="M39">
-        <v>9.376269088211077e-08</v>
+        <v>0.0001492270782217003</v>
       </c>
       <c r="N39">
         <v>0.0006026887372552962</v>
@@ -48502,7 +48502,7 @@
         <v>401</v>
       </c>
       <c r="M40">
-        <v>1.564013684462037e-07</v>
+        <v>0.0002490353822363803</v>
       </c>
       <c r="N40">
         <v>0.001706213228726593</v>
@@ -49704,7 +49704,7 @@
         <v>401</v>
       </c>
       <c r="M41">
-        <v>8.717527657391067e-09</v>
+        <v>2.416799400410647e-05</v>
       </c>
       <c r="N41">
         <v>1.054621927925451e-05</v>
@@ -50906,7 +50906,7 @@
         <v>401</v>
       </c>
       <c r="M42">
-        <v>1.373474857148412e-08</v>
+        <v>3.819660675493922e-05</v>
       </c>
       <c r="N42">
         <v>2.83287542015289e-05</v>
@@ -52108,7 +52108,7 @@
         <v>401</v>
       </c>
       <c r="M43">
-        <v>2.186030875168288e-08</v>
+        <v>6.080286131267009e-05</v>
       </c>
       <c r="N43">
         <v>7.488411896368258e-05</v>
@@ -53310,7 +53310,7 @@
         <v>401</v>
       </c>
       <c r="M44">
-        <v>3.50522903690606e-08</v>
+        <v>9.745495705817524e-05</v>
       </c>
       <c r="N44">
         <v>0.0001976732494618774</v>
@@ -54512,7 +54512,7 @@
         <v>401</v>
       </c>
       <c r="M45">
-        <v>5.708903478989548e-08</v>
+        <v>0.0001586275284062626</v>
       </c>
       <c r="N45">
         <v>0.0005263222830172438</v>
@@ -55714,7 +55714,7 @@
         <v>401</v>
       </c>
       <c r="M46">
-        <v>9.566158249071487e-08</v>
+        <v>0.0002657352886072652</v>
       </c>
       <c r="N46">
         <v>0.001440717543915689</v>
@@ -56916,7 +56916,7 @@
         <v>401</v>
       </c>
       <c r="M47">
-        <v>8.511508286093118e-09</v>
+        <v>4.229646762040637e-05</v>
       </c>
       <c r="N47">
         <v>2.494185122632942e-05</v>
@@ -58118,7 +58118,7 @@
         <v>401</v>
       </c>
       <c r="M48">
-        <v>1.384701841062612e-08</v>
+        <v>6.881168572627904e-05</v>
       </c>
       <c r="N48">
         <v>6.518189360176071e-05</v>
@@ -59320,7 +59320,7 @@
         <v>401</v>
       </c>
       <c r="M49">
-        <v>2.256677338108064e-08</v>
+        <v>0.0001121349682789465</v>
       </c>
       <c r="N49">
         <v>0.0001698376002395981</v>
@@ -60522,7 +60522,7 @@
         <v>401</v>
       </c>
       <c r="M50">
-        <v>3.70113458443762e-08</v>
+        <v>0.0001839982542220601</v>
       </c>
       <c r="N50">
         <v>0.0004438469737982759</v>
@@ -61724,7 +61724,7 @@
         <v>401</v>
       </c>
       <c r="M51">
-        <v>6.173855682752432e-08</v>
+        <v>0.0003072381262019005</v>
       </c>
       <c r="N51">
         <v>0.001178008751417075</v>
@@ -62926,7 +62926,7 @@
         <v>401</v>
       </c>
       <c r="M52">
-        <v>1.06209064214534e-07</v>
+        <v>0.0005297828366800253</v>
       </c>
       <c r="N52">
         <v>0.003232787786932274</v>
@@ -64128,7 +64128,7 @@
         <v>401</v>
       </c>
       <c r="M53">
-        <v>1.09636877741185e-08</v>
+        <v>0.0001011356717912024</v>
       </c>
       <c r="N53">
         <v>5.527546646859369e-05</v>
@@ -65330,7 +65330,7 @@
         <v>401</v>
       </c>
       <c r="M54">
-        <v>1.83365126401654e-08</v>
+        <v>0.0001700929403143556</v>
       </c>
       <c r="N54">
         <v>0.0001421236138808292</v>
@@ -66532,7 +66532,7 @@
         <v>401</v>
       </c>
       <c r="M55">
-        <v>3.068729361281062e-08</v>
+        <v>0.0002860979904335299</v>
       </c>
       <c r="N55">
         <v>0.0003666967004329113</v>
@@ -67734,7 +67734,7 @@
         <v>401</v>
       </c>
       <c r="M56">
-        <v>5.175561538343299e-08</v>
+        <v>0.0004846908644000164</v>
       </c>
       <c r="N56">
         <v>0.0009558611297395285</v>
@@ -68936,7 +68936,7 @@
         <v>401</v>
       </c>
       <c r="M57">
-        <v>8.921614222790255e-08</v>
+        <v>0.0008388583348068716</v>
       </c>
       <c r="N57">
         <v>0.002549850695894356</v>
@@ -70138,7 +70138,7 @@
         <v>401</v>
       </c>
       <c r="M58">
-        <v>1.619198823908244e-07</v>
+        <v>0.001523752910881625</v>
       </c>
       <c r="N58">
         <v>0.007012921292935432</v>

</xml_diff>